<commit_message>
update threshold and results
</commit_message>
<xml_diff>
--- a/tables/main_analyses_results.xlsx
+++ b/tables/main_analyses_results.xlsx
@@ -8,14 +8,15 @@
   <sheets>
     <sheet name="Model-Selection" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Coefficients" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Performance" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Classification-Table" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Final-Model" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Performance" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Risk-Table" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t xml:space="preserve">variable</t>
   </si>
@@ -122,7 +123,7 @@
     <t xml:space="preserve">selected_model</t>
   </si>
   <si>
-    <t xml:space="preserve">boot50_model</t>
+    <t xml:space="preserve">boot_model</t>
   </si>
   <si>
     <t xml:space="preserve">coef_shrink</t>
@@ -140,6 +141,36 @@
     <t xml:space="preserve">Intercept</t>
   </si>
   <si>
+    <t xml:space="preserve">boot_est</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boot_se</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drughx=Former</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drughx=Current</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_group=25-35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_group=35-45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_group=45-55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_group=55+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smokhx=Former</t>
+  </si>
+  <si>
+    <t xml:space="preserve">smokhx=Current</t>
+  </si>
+  <si>
     <t xml:space="preserve">stat</t>
   </si>
   <si>
@@ -185,7 +216,10 @@
     <t xml:space="preserve">brier_score</t>
   </si>
   <si>
-    <t xml:space="preserve">0.137</t>
+    <t xml:space="preserve">0.146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.144</t>
   </si>
   <si>
     <t xml:space="preserve">0.138</t>
@@ -194,43 +228,64 @@
     <t xml:space="preserve">0.145</t>
   </si>
   <si>
+    <t xml:space="preserve">0.140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.141</t>
+  </si>
+  <si>
     <t xml:space="preserve">cal_slope</t>
   </si>
   <si>
-    <t xml:space="preserve">1.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.966</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.994</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.786</t>
+    <t xml:space="preserve"> 0.8364</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.8861</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.1396</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.8964</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.0109</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0418</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.7253</t>
   </si>
   <si>
     <t xml:space="preserve">cal_int</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.000</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.004</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.024</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1.002</t>
+    <t xml:space="preserve">-0.177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.112</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.972</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.118</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.075</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.968</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.029</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.585</t>
   </si>
   <si>
     <t xml:space="preserve">c_ci</t>
@@ -239,49 +294,46 @@
     <t xml:space="preserve">0.78 (0.74, 0.81)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.74 (0.7, 0.78)</t>
+    <t xml:space="preserve">0.77 (0.73, 0.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.76 (0.72, 0.79)</t>
   </si>
   <si>
     <t xml:space="preserve">risk_group</t>
   </si>
   <si>
-    <t xml:space="preserve">max_pred_val</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_below_cut_off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">perc_below_cut_off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cm_outcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cm_no_outcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sensitivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">specificity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ppv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">npv</t>
+    <t xml:space="preserve">min_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max_score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">risk_cut_off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prop_group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obs_prob_outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pred_prob_outcome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Low risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High risk</t>
   </si>
 </sst>
 </file>
@@ -1475,19 +1527,19 @@
         <v>0.9182</v>
       </c>
       <c r="E2" t="n">
-        <v>0.908870414360167</v>
+        <v>0.655182554952949</v>
       </c>
       <c r="F2" t="n">
-        <v>0.808935243022191</v>
+        <v>0.596891473085308</v>
       </c>
       <c r="G2" t="n">
-        <v>0.906747396191383</v>
+        <v>0.62017244207942</v>
       </c>
       <c r="H2" t="n">
-        <v>0.898208960400552</v>
+        <v>0.864851716230745</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.268608043340789</v>
+        <v>0.058185938292088</v>
       </c>
     </row>
     <row r="3">
@@ -1504,19 +1556,19 @@
         <v>-0.1783</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.170947880547651</v>
+        <v>-0.178620636541701</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.15215124522707</v>
+        <v>-0.162728897561181</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.172333313593026</v>
+        <v>-0.177174795118711</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.16911623136707</v>
+        <v>-0.166422340788736</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.10850030852946</v>
+        <v>-0.121103143941974</v>
       </c>
     </row>
     <row r="4">
@@ -1533,19 +1585,19 @@
         <v>0.7803</v>
       </c>
       <c r="E4" t="n">
-        <v>0.78019549595202</v>
+        <v>0.706347490884611</v>
       </c>
       <c r="F4" t="n">
-        <v>0.694408821269721</v>
+        <v>0.64350430449801</v>
       </c>
       <c r="G4" t="n">
-        <v>0.782682269946239</v>
+        <v>0.743330271149772</v>
       </c>
       <c r="H4" t="n">
-        <v>0.767414754651669</v>
+        <v>0.752869448227628</v>
       </c>
       <c r="I4" t="n">
-        <v>0.403616808268719</v>
+        <v>0.448373056781211</v>
       </c>
     </row>
     <row r="5">
@@ -1562,19 +1614,19 @@
         <v>0.4369</v>
       </c>
       <c r="E5" t="n">
-        <v>0.40167990879821</v>
+        <v>0.496993364454314</v>
       </c>
       <c r="F5" t="n">
-        <v>0.357513050823158</v>
+        <v>0.452776251718214</v>
       </c>
       <c r="G5" t="n">
-        <v>0.403880953595245</v>
+        <v>0.517240165642722</v>
       </c>
       <c r="H5" t="n">
-        <v>0.403600862870935</v>
+        <v>0.409718548281497</v>
       </c>
       <c r="I5" t="n">
-        <v>0.245399141173057</v>
+        <v>0.28722022218609</v>
       </c>
     </row>
     <row r="6">
@@ -1591,19 +1643,19 @@
         <v>1.157</v>
       </c>
       <c r="E6" t="n">
-        <v>1.12433164118783</v>
+        <v>1.18857487343604</v>
       </c>
       <c r="F6" t="n">
-        <v>1.00070535362525</v>
+        <v>1.08282829222822</v>
       </c>
       <c r="G6" t="n">
-        <v>1.12783970196376</v>
+        <v>1.21447076193714</v>
       </c>
       <c r="H6" t="n">
-        <v>1.1032364500574</v>
+        <v>1.11130768769328</v>
       </c>
       <c r="I6" t="n">
-        <v>0.884371112989442</v>
+        <v>0.971340920417073</v>
       </c>
     </row>
     <row r="7">
@@ -1620,19 +1672,19 @@
         <v>0.7006</v>
       </c>
       <c r="E7" t="n">
-        <v>0.690206583942606</v>
+        <v>0.654327441716923</v>
       </c>
       <c r="F7" t="n">
-        <v>0.614314672251915</v>
+        <v>0.596112438608203</v>
       </c>
       <c r="G7" t="n">
-        <v>0.689446117984269</v>
+        <v>0.660450197919444</v>
       </c>
       <c r="H7" t="n">
-        <v>0.675860104272029</v>
+        <v>0.650435973524505</v>
       </c>
       <c r="I7" t="n">
-        <v>0.131522491942062</v>
+        <v>0.244966315984164</v>
       </c>
     </row>
     <row r="8">
@@ -1649,16 +1701,16 @@
         <v>-0.4557</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.44438040258064</v>
+        <v>-0.481533801415784</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.395518396546041</v>
+        <v>-0.438692113968261</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.45286959412348</v>
+        <v>-0.504265650131965</v>
       </c>
       <c r="H8" t="n">
-        <v>-0.399659048870074</v>
+        <v>-0.342429704261508</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -1678,16 +1730,16 @@
         <v>-0.6709</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.643917191641829</v>
+        <v>-0.705330149181666</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.573115046630325</v>
+        <v>-0.642577474894396</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.653479588461276</v>
+        <v>-0.728324082059197</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.584963856051204</v>
+        <v>-0.515609363906703</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1707,19 +1759,19 @@
         <v>-1.1024</v>
       </c>
       <c r="E10" t="n">
-        <v>-1.06350355825461</v>
+        <v>-1.0856376757826</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.946565644297382</v>
+        <v>-0.989049336915456</v>
       </c>
       <c r="G10" t="n">
-        <v>-1.08836592131008</v>
+        <v>-1.11967840447223</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.990294249709928</v>
+        <v>-0.911470231304127</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.00951772854814628</v>
+        <v>-0.143382975682025</v>
       </c>
     </row>
     <row r="11">
@@ -1736,16 +1788,16 @@
         <v>-0.3533</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.432729477913166</v>
+        <v>-0.458173412723236</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.385148553465659</v>
+        <v>-0.417410080872093</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.441938565492124</v>
+        <v>-0.475356131193776</v>
       </c>
       <c r="H11" t="n">
-        <v>-0.301487122744513</v>
+        <v>-0.230306197863567</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1765,19 +1817,19 @@
         <v>-0.0598</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.054678765778601</v>
+        <v>-0.0575942613304553</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.0486665425394054</v>
+        <v>-0.0524701447358659</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.0548603579401968</v>
+        <v>-0.0615136027128685</v>
       </c>
       <c r="H12" t="n">
-        <v>-0.0543222455294945</v>
+        <v>-0.0517476642586506</v>
       </c>
       <c r="I12" t="n">
-        <v>-0.0177912976421618</v>
+        <v>-0.0248094573989105</v>
       </c>
     </row>
     <row r="13">
@@ -1794,19 +1846,19 @@
         <v>0.6162</v>
       </c>
       <c r="E13" t="n">
-        <v>0.590396257839289</v>
+        <v>0.633493681932743</v>
       </c>
       <c r="F13" t="n">
-        <v>0.52547902623812</v>
+        <v>0.577132242213355</v>
       </c>
       <c r="G13" t="n">
-        <v>0.597681433502853</v>
+        <v>0.653316131571823</v>
       </c>
       <c r="H13" t="n">
-        <v>0.570970939327537</v>
+        <v>0.559063325841032</v>
       </c>
       <c r="I13" t="n">
-        <v>0.153289637227175</v>
+        <v>0.219821154348321</v>
       </c>
     </row>
     <row r="14">
@@ -1823,19 +1875,19 @@
         <v>0.4924</v>
       </c>
       <c r="E14" t="n">
-        <v>0.484093692146602</v>
+        <v>0.555038102032423</v>
       </c>
       <c r="F14" t="n">
-        <v>0.430864997160022</v>
+        <v>0.505656794180667</v>
       </c>
       <c r="G14" t="n">
-        <v>0.486679437432394</v>
+        <v>0.592307786547246</v>
       </c>
       <c r="H14" t="n">
-        <v>0.448473080409222</v>
+        <v>0.431166521238387</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>0.037324465698089</v>
       </c>
     </row>
     <row r="15">
@@ -1852,19 +1904,19 @@
         <v>-0.368</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.356382341635706</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.317196193852179</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.363111665882274</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>-0.320403691127748</v>
+        <v>-0.309259108157208</v>
       </c>
       <c r="I15" t="n">
-        <v>-0.0107453859117379</v>
+        <v>-0.0840181081151429</v>
       </c>
     </row>
     <row r="16">
@@ -1881,19 +1933,19 @@
         <v>-0.0477</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.0433738625628156</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.0386046739982871</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.0425939638319347</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>-0.0441998405393962</v>
+        <v>-0.0433722092409604</v>
       </c>
       <c r="I16" t="n">
-        <v>-0.00150854158551117</v>
+        <v>-0.0132493989877956</v>
       </c>
     </row>
     <row r="17">
@@ -1910,16 +1962,16 @@
         <v>0.3792</v>
       </c>
       <c r="E17" t="n">
-        <v>0.370216648657101</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.329509344699182</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.375854791687083</v>
+        <v>0</v>
       </c>
       <c r="H17" t="n">
-        <v>0.347624339756366</v>
+        <v>0.326228660543763</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
@@ -1939,19 +1991,19 @@
         <v>0.3895</v>
       </c>
       <c r="E18" t="n">
-        <v>0.392438687822673</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.349287951603783</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.393922394578954</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0.339779415367445</v>
+        <v>0.326143405343783</v>
       </c>
       <c r="I18" t="n">
-        <v>0.00185064848341526</v>
+        <v>0.0771984508296663</v>
       </c>
     </row>
     <row r="19">
@@ -1977,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.227638073041648</v>
+        <v>-0.212068824984202</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
@@ -2006,7 +2058,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>-0.202574461037054</v>
+        <v>-0.19340528043643</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
@@ -2035,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0897266097358721</v>
+        <v>0.034299942346324</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
@@ -2064,7 +2116,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>0.129534661762851</v>
+        <v>0.0748999566963938</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
@@ -2093,7 +2145,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.0129026748267102</v>
+        <v>-0.00386773235796934</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -2115,176 +2167,156 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>54</v>
+        <v>40</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.655182554952949</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.63163948975285</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" t="s">
-        <v>58</v>
+        <v>12</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-0.178620636541701</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.0456741631891731</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" t="s">
-        <v>64</v>
-      </c>
-      <c r="I4" t="s">
-        <v>65</v>
+        <v>13</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.706347490884611</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.222844217051302</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" t="s">
-        <v>71</v>
+        <v>43</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.496993364454314</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.238522798726937</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" t="s">
-        <v>74</v>
+        <v>44</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1.18857487343604</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.280452557197171</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.654327441716923</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.205314101326851</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-0.481533801415784</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.253932696183804</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-0.705330149181666</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.272567604157862</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-1.0856376757826</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.329973922580573</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="n">
+        <v>-0.458173412723236</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.320680650513755</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="n">
+        <v>-0.0575942613304553</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0232763885385104</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.633493681932743</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.22737834491918</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.555038102032423</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.254994470874304</v>
       </c>
     </row>
   </sheetData>
@@ -2303,486 +2335,306 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
         <v>75</v>
       </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="s">
+        <v>92</v>
+      </c>
+      <c r="H6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="H1" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="I1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L1" t="s">
-        <v>86</v>
-      </c>
-      <c r="M1" t="s">
-        <v>87</v>
-      </c>
-      <c r="N1" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>103</v>
       </c>
       <c r="B2" t="n">
-        <v>-2.96138046294369</v>
+        <v>-6.93471322189013</v>
       </c>
       <c r="C2" t="n">
-        <v>95</v>
+        <v>-2.1972582831671</v>
       </c>
       <c r="D2" t="n">
-        <v>0.100635593220339</v>
+        <v>-2.1972582831671</v>
       </c>
       <c r="E2" t="n">
-        <v>3</v>
+        <v>307</v>
       </c>
       <c r="F2" t="n">
-        <v>92</v>
+        <v>0.32521186440678</v>
       </c>
       <c r="G2" t="n">
-        <v>188</v>
+        <v>13</v>
       </c>
       <c r="H2" t="n">
-        <v>92</v>
+        <v>0.0423452768729642</v>
       </c>
       <c r="I2" t="n">
-        <v>661</v>
-      </c>
-      <c r="J2" t="n">
-        <v>3</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.984293193717278</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.122177954847278</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.221436984687868</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.968421052631579</v>
+        <v>0.0672323809918907</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
+      <c r="A3" t="s">
+        <v>104</v>
       </c>
       <c r="B3" t="n">
-        <v>-2.57594908337959</v>
+        <v>-2.19325021279916</v>
       </c>
       <c r="C3" t="n">
-        <v>190</v>
+        <v>-1.38680362030269</v>
       </c>
       <c r="D3" t="n">
-        <v>0.201271186440678</v>
+        <v>-1.38680362030269</v>
       </c>
       <c r="E3" t="n">
-        <v>6</v>
+        <v>277</v>
       </c>
       <c r="F3" t="n">
-        <v>184</v>
+        <v>0.293432203389831</v>
       </c>
       <c r="G3" t="n">
-        <v>185</v>
+        <v>47</v>
       </c>
       <c r="H3" t="n">
-        <v>184</v>
+        <v>0.169675090252708</v>
       </c>
       <c r="I3" t="n">
-        <v>569</v>
-      </c>
-      <c r="J3" t="n">
-        <v>6</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.968586387434555</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.244355909694555</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.245358090185676</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.968421052631579</v>
+        <v>0.145853979361813</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
+      <c r="A4" t="s">
+        <v>105</v>
       </c>
       <c r="B4" t="n">
-        <v>-2.2943395380321</v>
+        <v>-1.3813601067548</v>
       </c>
       <c r="C4" t="n">
-        <v>285</v>
+        <v>1.34821931050698</v>
       </c>
       <c r="D4" t="n">
-        <v>0.301906779661017</v>
+        <v>1.34821931050698</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>360</v>
       </c>
       <c r="F4" t="n">
-        <v>275</v>
+        <v>0.38135593220339</v>
       </c>
       <c r="G4" t="n">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="H4" t="n">
-        <v>275</v>
+        <v>0.363888888888889</v>
       </c>
       <c r="I4" t="n">
-        <v>478</v>
-      </c>
-      <c r="J4" t="n">
-        <v>10</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.947643979057592</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.365205843293493</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.274658573596358</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.964912280701754</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>-1.9993977075351</v>
-      </c>
-      <c r="C5" t="n">
-        <v>380</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.402542372881356</v>
-      </c>
-      <c r="E5" t="n">
-        <v>20</v>
-      </c>
-      <c r="F5" t="n">
-        <v>360</v>
-      </c>
-      <c r="G5" t="n">
-        <v>171</v>
-      </c>
-      <c r="H5" t="n">
-        <v>360</v>
-      </c>
-      <c r="I5" t="n">
-        <v>393</v>
-      </c>
-      <c r="J5" t="n">
-        <v>20</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.895287958115183</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.47808764940239</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.303191489361702</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.947368421052632</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>-1.70470506459454</v>
-      </c>
-      <c r="C6" t="n">
-        <v>474</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.502118644067797</v>
-      </c>
-      <c r="E6" t="n">
-        <v>31</v>
-      </c>
-      <c r="F6" t="n">
-        <v>443</v>
-      </c>
-      <c r="G6" t="n">
-        <v>160</v>
-      </c>
-      <c r="H6" t="n">
-        <v>443</v>
-      </c>
-      <c r="I6" t="n">
-        <v>310</v>
-      </c>
-      <c r="J6" t="n">
-        <v>31</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.837696335078534</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.588313413014608</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.340425531914894</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.934599156118143</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>-1.42860339540503</v>
-      </c>
-      <c r="C7" t="n">
-        <v>568</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.601694915254237</v>
-      </c>
-      <c r="E7" t="n">
-        <v>54</v>
-      </c>
-      <c r="F7" t="n">
-        <v>514</v>
-      </c>
-      <c r="G7" t="n">
-        <v>137</v>
-      </c>
-      <c r="H7" t="n">
-        <v>514</v>
-      </c>
-      <c r="I7" t="n">
-        <v>239</v>
-      </c>
-      <c r="J7" t="n">
-        <v>54</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.717277486910995</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.682602921646746</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.36436170212766</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.904929577464789</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>-1.11425661364234</v>
-      </c>
-      <c r="C8" t="n">
-        <v>662</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.701271186440678</v>
-      </c>
-      <c r="E8" t="n">
-        <v>72</v>
-      </c>
-      <c r="F8" t="n">
-        <v>590</v>
-      </c>
-      <c r="G8" t="n">
-        <v>119</v>
-      </c>
-      <c r="H8" t="n">
-        <v>590</v>
-      </c>
-      <c r="I8" t="n">
-        <v>163</v>
-      </c>
-      <c r="J8" t="n">
-        <v>72</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.62303664921466</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.783532536520584</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.421985815602837</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.891238670694864</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>-0.784406994395853</v>
-      </c>
-      <c r="C9" t="n">
-        <v>756</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.800847457627119</v>
-      </c>
-      <c r="E9" t="n">
-        <v>103</v>
-      </c>
-      <c r="F9" t="n">
-        <v>653</v>
-      </c>
-      <c r="G9" t="n">
-        <v>88</v>
-      </c>
-      <c r="H9" t="n">
-        <v>653</v>
-      </c>
-      <c r="I9" t="n">
-        <v>100</v>
-      </c>
-      <c r="J9" t="n">
-        <v>103</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.460732984293194</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.867197875166003</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.468085106382979</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.863756613756614</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>-0.29398842819021</v>
-      </c>
-      <c r="C10" t="n">
-        <v>850</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.900423728813559</v>
-      </c>
-      <c r="E10" t="n">
-        <v>143</v>
-      </c>
-      <c r="F10" t="n">
-        <v>707</v>
-      </c>
-      <c r="G10" t="n">
-        <v>48</v>
-      </c>
-      <c r="H10" t="n">
-        <v>707</v>
-      </c>
-      <c r="I10" t="n">
-        <v>46</v>
-      </c>
-      <c r="J10" t="n">
-        <v>143</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.25130890052356</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.938911022576361</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.51063829787234</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.831764705882353</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1.65376424318962</v>
-      </c>
-      <c r="C11" t="n">
-        <v>944</v>
-      </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>191</v>
-      </c>
-      <c r="F11" t="n">
-        <v>753</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>753</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>191</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" t="n">
-        <v>1</v>
-      </c>
-      <c r="M11" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.797669491525424</v>
+        <v>0.360994740978521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>